<commit_message>
Added filter button, working on adding integrated db
</commit_message>
<xml_diff>
--- a/docs/planning.xlsx
+++ b/docs/planning.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9096"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9096" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>User</t>
   </si>
@@ -69,6 +70,21 @@
   </si>
   <si>
     <t>Card Viewer</t>
+  </si>
+  <si>
+    <t>uuid</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>variation json</t>
+  </si>
+  <si>
+    <t>detail json</t>
+  </si>
+  <si>
+    <t>image blob</t>
   </si>
 </sst>
 </file>
@@ -789,8 +805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -891,4 +907,41 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="14.109375" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>